<commit_message>
added images chart png
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arash\Desktop\Web dev minor\project-2-1819\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE19FC62-C246-4DBC-8F22-E56D9330B97F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E62823-8B0E-4DF0-8C20-6806EE72D8E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{49D6E8A7-ABD9-443A-B770-62FFA2878FBB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Gzip</t>
   </si>
@@ -66,13 +66,23 @@
   <si>
     <t>Original</t>
   </si>
+  <si>
+    <t>Total size of 7 images</t>
+  </si>
+  <si>
+    <t>Original (jpeg and png)</t>
+  </si>
+  <si>
+    <t>WebP version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0\ &quot;KB&quot;"/>
+    <numFmt numFmtId="175" formatCode="0.0#\ &quot;MB&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -103,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1207,11 +1218,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$1</c:f>
+              <c:f>Blad3!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzip</c:v>
+                  <c:v>Original (jpeg and png)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1285,35 +1296,23 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$2:$A$4</c:f>
+              <c:f>Blad3!$A$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>homepage</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>styles.min.css</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>scripts.min.js</c:v>
+                  <c:v>Total size of 7 images</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$2:$B$4</c:f>
+              <c:f>Blad3!$B$2</c:f>
               <c:numCache>
-                <c:formatCode>0\ "KB"</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>0.0#\ "MB"</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>4.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1329,11 +1328,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$C$1</c:f>
+              <c:f>Blad3!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Brotli</c:v>
+                  <c:v>WebP version</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1407,35 +1406,23 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad1!$A$2:$A$4</c:f>
+              <c:f>Blad3!$A$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>homepage</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>styles.min.css</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>scripts.min.js</c:v>
+                  <c:v>Total size of 7 images</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$2:$C$4</c:f>
+              <c:f>Blad3!$C$2</c:f>
               <c:numCache>
-                <c:formatCode>0\ "KB"</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>0.0#\ "MB"</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>1.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,7 +1518,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0\ &quot;KB&quot;" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0#\ &quot;MB&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3370,10 +3357,10 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>17379</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3839,7 +3826,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3851,47 +3838,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
-      <c r="B2" s="1">
-        <v>144</v>
+      <c r="B2" s="2">
+        <v>4.43</v>
       </c>
-      <c r="C2" s="1">
-        <v>123</v>
+      <c r="C2" s="2">
+        <v>1.27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>35</v>
-      </c>
-      <c r="C3" s="1">
-        <v>28</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1">
-        <v>15</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>